<commit_message>
Added new crops dataset from FAO, identified high-yield crops in low-producing countries
</commit_message>
<xml_diff>
--- a/T-Test_Results.xlsx
+++ b/T-Test_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University Studies\Spring 2023\Independent Study Revival\Github\Agriculture-Data-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44CE744-DE25-46FD-AB39-D31828BE00E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58FA791-6E91-48FD-9FD1-9549F57F9306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -458,8 +458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>